<commit_message>
completed SavingsAccount and tests
</commit_message>
<xml_diff>
--- a/tests/A02_pixell_test_plan_investment_account.xlsx
+++ b/tests/A02_pixell_test_plan_investment_account.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ADD\Term2\intermediate_software_development\project\Assignment_01\isd_project\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DECBFB-3643-4BDE-AAF6-00EAC1785127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34C6D8B-5A1F-4B5E-89E6-6A864D667078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="90" windowWidth="18398" windowHeight="12480" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1189,7 +1189,7 @@
   <dimension ref="B1:G34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>